<commit_message>
add ON_STARTUP promt with proper scope on callback
</commit_message>
<xml_diff>
--- a/design/prompts.xlsx
+++ b/design/prompts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15940" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22620" windowHeight="9780" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="30">
   <si>
     <t>Location</t>
   </si>
@@ -51,9 +51,6 @@
     <t>PICK_UP_IPAD</t>
   </si>
   <si>
-    <t>[partner] pick up the iPad and hold it so you can see my face but your partner can't.</t>
-  </si>
-  <si>
     <t>READ_THE_WORD</t>
   </si>
   <si>
@@ -75,28 +72,43 @@
     <t>Turn me over please!</t>
   </si>
   <si>
-    <t>[partner] find the word your partner read to you and tap it with your finger.</t>
-  </si>
-  <si>
-    <t>ON_CORRECT_SELECTION</t>
-  </si>
-  <si>
     <t>ON_STARTUP</t>
   </si>
   <si>
     <t>ON_INTRO</t>
   </si>
   <si>
-    <t>ON_SELECT_STIMULUS</t>
-  </si>
-  <si>
-    <t>ON_INCORRECT_SELECTION</t>
-  </si>
-  <si>
     <t>[partner] the word you chose was [ANSWER]</t>
   </si>
   <si>
-    <t>[partner] The right answer weas [ANSWER]</t>
+    <t>[partner] The right answer was [ANSWER]</t>
+  </si>
+  <si>
+    <t>:</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t>//</t>
+  </si>
+  <si>
+    <t>"</t>
+  </si>
+  <si>
+    <t>[partner] now pick up the iPad and hold it so you can see my face but your partner can't.</t>
+  </si>
+  <si>
+    <t>[partner ]now find the word your partner read to you and tap it with your finger.</t>
+  </si>
+  <si>
+    <t>SELECT_STIMULUS</t>
+  </si>
+  <si>
+    <t>CORRECT_STIMULUS</t>
+  </si>
+  <si>
+    <t>INCORRECT_SELECTION</t>
   </si>
 </sst>
 </file>
@@ -145,8 +157,42 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -156,9 +202,43 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="37">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -488,123 +568,340 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="40.83203125" customWidth="1"/>
-    <col min="2" max="2" width="80.33203125" style="1" customWidth="1"/>
+    <col min="2" max="3" width="2.1640625" customWidth="1"/>
+    <col min="4" max="4" width="28.5" customWidth="1"/>
+    <col min="5" max="5" width="2.1640625" customWidth="1"/>
+    <col min="6" max="7" width="4.6640625" customWidth="1"/>
+    <col min="8" max="8" width="80.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="56" customHeight="1">
+    <row r="1" spans="1:8" ht="56" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="24" customHeight="1">
+    <row r="2" spans="1:8" ht="24" customHeight="1">
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="30">
+    <row r="4" spans="1:8" ht="30">
       <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="1" t="s">
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="20" customHeight="1"/>
+    </row>
+    <row r="16" spans="1:8" ht="20" customHeight="1"/>
     <row r="20" ht="18" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
add audios clean up prompt
</commit_message>
<xml_diff>
--- a/design/prompts.xlsx
+++ b/design/prompts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22620" windowHeight="9780" tabRatio="500"/>
+    <workbookView xWindow="4840" yWindow="-15260" windowWidth="22620" windowHeight="11960" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="42">
   <si>
     <t>Location</t>
   </si>
@@ -33,30 +33,12 @@
     <t>This game will help you learn with your partner. One of you will be the red partner and one will be the blue partner. You decide!</t>
   </si>
   <si>
-    <t>Blue Partner</t>
-  </si>
-  <si>
-    <t>Red Partner</t>
-  </si>
-  <si>
     <t>ON_VERTICAL_STARTUP</t>
   </si>
   <si>
-    <t>BLUE_PARTNER</t>
-  </si>
-  <si>
-    <t>RED_PARTNER</t>
-  </si>
-  <si>
-    <t>PICK_UP_IPAD</t>
-  </si>
-  <si>
     <t>READ_THE_WORD</t>
   </si>
   <si>
-    <t xml:space="preserve">Great! Now read the word you see out loud so your partner can hear it. </t>
-  </si>
-  <si>
     <t>PUT_DOWN_THE_IPAD</t>
   </si>
   <si>
@@ -66,49 +48,103 @@
     <t>When you have read the word, place the iPad flat in front of you again.</t>
   </si>
   <si>
-    <t>ON_SCREEN_FACING_DOWN</t>
-  </si>
-  <si>
-    <t>Turn me over please!</t>
-  </si>
-  <si>
     <t>ON_STARTUP</t>
   </si>
   <si>
     <t>ON_INTRO</t>
   </si>
   <si>
-    <t>[partner] the word you chose was [ANSWER]</t>
-  </si>
-  <si>
-    <t>[partner] The right answer was [ANSWER]</t>
-  </si>
-  <si>
-    <t>:</t>
-  </si>
-  <si>
-    <t>,</t>
-  </si>
-  <si>
     <t>//</t>
   </si>
   <si>
     <t>"</t>
   </si>
   <si>
-    <t>[partner] now pick up the iPad and hold it so you can see my face but your partner can't.</t>
-  </si>
-  <si>
-    <t>[partner ]now find the word your partner read to you and tap it with your finger.</t>
-  </si>
-  <si>
-    <t>SELECT_STIMULUS</t>
-  </si>
-  <si>
     <t>CORRECT_STIMULUS</t>
   </si>
   <si>
     <t>INCORRECT_SELECTION</t>
+  </si>
+  <si>
+    <t>RED_PICK_UP_IPAD</t>
+  </si>
+  <si>
+    <t>BLUE_PICK_UP_IPAD</t>
+  </si>
+  <si>
+    <t>Red partner now pick up the iPad and hold it so you can see my face but your partner can't.</t>
+  </si>
+  <si>
+    <t>Blue partner now pick up the iPad and hold it so you can see my face but your partner can't.</t>
+  </si>
+  <si>
+    <t>RED_SELECT_STIMULUS</t>
+  </si>
+  <si>
+    <t>BLUE_SELECT_STIMULUS</t>
+  </si>
+  <si>
+    <t>Red partner now find the word your partner read to you and tap it with your finger.</t>
+  </si>
+  <si>
+    <t>Blue partner now find the word your partner read to you and tap it with your finger.</t>
+  </si>
+  <si>
+    <t>CORRECT_SELECTION</t>
+  </si>
+  <si>
+    <t>The right answer was [ANSWER]</t>
+  </si>
+  <si>
+    <t>The word you chose was [ANSWER]</t>
+  </si>
+  <si>
+    <t>Great! The right answer was [ANSWER]</t>
+  </si>
+  <si>
+    <t>Great! Now read the word you see out loud so your partner can hear it. When you have read the word, place the iPad flat in front of you again.</t>
+  </si>
+  <si>
+    <t>p_ON_INTRO</t>
+  </si>
+  <si>
+    <t>p_ON_VERTICAL_STARTUP</t>
+  </si>
+  <si>
+    <t>p_ON_STARTUP</t>
+  </si>
+  <si>
+    <t>p_RED_PICK_UP_IPAD</t>
+  </si>
+  <si>
+    <t>p_BLUE_PICK_UP_IPAD</t>
+  </si>
+  <si>
+    <t>p_READ_THE_WORD</t>
+  </si>
+  <si>
+    <t>p_PUT_DOWN_THE_IPAD</t>
+  </si>
+  <si>
+    <t>p_RED_SELECT_STIMULUS</t>
+  </si>
+  <si>
+    <t>p_BLUE_SELECT_STIMULUS</t>
+  </si>
+  <si>
+    <t>p_CORRECT_STIMULUS</t>
+  </si>
+  <si>
+    <t>p_INCORRECT_SELECTION</t>
+  </si>
+  <si>
+    <t>p_CORRECT_SELECTION</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>;</t>
   </si>
 </sst>
 </file>
@@ -157,8 +193,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -202,7 +246,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="45">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -221,6 +265,10 @@
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -239,6 +287,10 @@
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -568,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -594,51 +646,51 @@
     </row>
     <row r="2" spans="1:8" ht="24" customHeight="1">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="G2" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="G3" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>2</v>
@@ -646,25 +698,25 @@
     </row>
     <row r="4" spans="1:8" ht="30">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="G4" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>3</v>
@@ -672,237 +724,240 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="G5" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="G6" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="H6" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="30">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
       <c r="E7" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="G7" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="G8" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="C9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E10" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="G10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="D11" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" t="s">
-        <v>23</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="E12" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F12" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="G12" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E13" t="s">
-        <v>24</v>
+        <v>12</v>
+      </c>
+      <c r="F13" t="s">
+        <v>41</v>
       </c>
       <c r="G13" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="20" customHeight="1"/>
-    <row r="20" ht="18" customHeight="1"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="20" customHeight="1"/>
+    <row r="19" ht="18" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
add OnResume event processing
</commit_message>
<xml_diff>
--- a/design/prompts.xlsx
+++ b/design/prompts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4840" yWindow="-15260" windowWidth="22620" windowHeight="11960" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,9 +30,6 @@
     <t>Welcome to MC Partner. Is this the first time you have played? Tap the green Yes or the red No</t>
   </si>
   <si>
-    <t>This game will help you learn with your partner. One of you will be the red partner and one will be the blue partner. You decide!</t>
-  </si>
-  <si>
     <t>ON_VERTICAL_STARTUP</t>
   </si>
   <si>
@@ -72,12 +69,6 @@
     <t>BLUE_PICK_UP_IPAD</t>
   </si>
   <si>
-    <t>Red partner now pick up the iPad and hold it so you can see my face but your partner can't.</t>
-  </si>
-  <si>
-    <t>Blue partner now pick up the iPad and hold it so you can see my face but your partner can't.</t>
-  </si>
-  <si>
     <t>RED_SELECT_STIMULUS</t>
   </si>
   <si>
@@ -99,12 +90,6 @@
     <t>The word you chose was [ANSWER]</t>
   </si>
   <si>
-    <t>Great! The right answer was [ANSWER]</t>
-  </si>
-  <si>
-    <t>Great! Now read the word you see out loud so your partner can hear it. When you have read the word, place the iPad flat in front of you again.</t>
-  </si>
-  <si>
     <t>p_ON_INTRO</t>
   </si>
   <si>
@@ -145,6 +130,21 @@
   </si>
   <si>
     <t>;</t>
+  </si>
+  <si>
+    <t>Red partner, pick up the iPad and hold it in front of your face so your partner is looking at the back of the iPad.</t>
+  </si>
+  <si>
+    <t>Blue partner,  pick up the iPad and hold it in front of your face so your partner is looking at the back of the iPad.</t>
+  </si>
+  <si>
+    <t>OK, Now read the word you see out loud so your partner can hear it. When you have read the word, place the iPad flat in front of you again.</t>
+  </si>
+  <si>
+    <t>This game will help you and your partner learn to read. One of you will be the red partner and one will be the blue partner. You decide together who will be blue and who will be red!</t>
+  </si>
+  <si>
+    <t>You're right! The answer was [ANSWER]</t>
   </si>
 </sst>
 </file>
@@ -623,7 +623,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -646,51 +646,51 @@
     </row>
     <row r="2" spans="1:8" ht="24" customHeight="1">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>2</v>
@@ -698,262 +698,262 @@
     </row>
     <row r="4" spans="1:8" ht="30">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" t="s">
-        <v>41</v>
-      </c>
-      <c r="G4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+    </row>
+    <row r="5" spans="1:8" ht="30">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="30">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
         <v>15</v>
       </c>
-      <c r="E5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" t="s">
-        <v>41</v>
-      </c>
-      <c r="G5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="30">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F9" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F10" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
         <v>12</v>
       </c>
-      <c r="D11" t="s">
-        <v>13</v>
-      </c>
       <c r="E11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F12" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="G13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="20" customHeight="1"/>

</xml_diff>